<commit_message>
No rounding on 1 decimal
</commit_message>
<xml_diff>
--- a/src/test/resources/Student Profile.xlsx
+++ b/src/test/resources/Student Profile.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\excel-parser\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="29740" yWindow="1180" windowWidth="25520" windowHeight="15560" tabRatio="78"/>
+    <workbookView xWindow="29745" yWindow="1185" windowWidth="25515" windowHeight="15555" tabRatio="78"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -185,6 +190,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -513,24 +526,24 @@
   <dimension ref="A2:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,7 +551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -546,7 +559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -578,7 +591,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -608,7 +621,7 @@
         <v>37539.375</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -631,7 +644,7 @@
         <v>18</v>
       </c>
       <c r="H7" s="2">
-        <v>450.3</v>
+        <v>450.35</v>
       </c>
       <c r="I7" s="6">
         <v>37540</v>
@@ -640,7 +653,7 @@
         <v>37540.416666666664</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -693,7 +706,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -715,7 +728,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>